<commit_message>
Added motor_type and all mods.  Need Help details
</commit_message>
<xml_diff>
--- a/help.xlsx
+++ b/help.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{230FC70D-A2A1-48E6-92AD-BDC882185FDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="0" windowWidth="28800" windowHeight="16520"/>
+    <workbookView xWindow="825" yWindow="540" windowWidth="27675" windowHeight="11790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Import-Export Sheet" sheetId="1" r:id="rId1"/>
@@ -20,12 +21,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="C3" authorId="0">
+    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -49,7 +50,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D3" authorId="0">
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -75,7 +76,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E3" authorId="0">
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -101,7 +102,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F3" authorId="0">
+    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -130,7 +131,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G3" authorId="0">
+    <comment ref="G3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -158,7 +159,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H3" authorId="0">
+    <comment ref="H3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -182,7 +183,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I3" authorId="0">
+    <comment ref="I3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -210,7 +211,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J3" authorId="0">
+    <comment ref="J3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -234,7 +235,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K3" authorId="0">
+    <comment ref="K3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -258,7 +259,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L3" authorId="0">
+    <comment ref="L3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -282,7 +283,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M3" authorId="0">
+    <comment ref="N3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -306,7 +307,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N3" authorId="0">
+    <comment ref="O3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -330,7 +331,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O3" authorId="0">
+    <comment ref="P3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -355,7 +356,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P3" authorId="0">
+    <comment ref="Q3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -379,7 +380,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q3" authorId="0">
+    <comment ref="R3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -403,7 +404,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AJ3" authorId="0">
+    <comment ref="AG3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
       <text>
         <r>
           <rPr>
@@ -427,7 +428,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AO3" authorId="0">
+    <comment ref="AL3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
       <text>
         <r>
           <rPr>
@@ -456,7 +457,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="123">
   <si>
     <t>Participant / Manufacturer</t>
   </si>
@@ -513,18 +514,6 @@
   </si>
   <si>
     <t>100% BEP Head</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pump Input Power @ 75% BEP </t>
-  </si>
-  <si>
-    <t>Pump Input Power @ 100% of BEP</t>
-  </si>
-  <si>
-    <t>Pump Input Power @ 110% of BEP</t>
-  </si>
-  <si>
-    <t>Pump Input Power @ 120% of BEP</t>
   </si>
   <si>
     <t xml:space="preserve">Driver Input Power @ 100% BEP </t>
@@ -600,12 +589,6 @@
   </si>
   <si>
     <t>On import, only use the 100% BEP flow point.  The other load points will be automatically calculated.</t>
-  </si>
-  <si>
-    <t>Section 3, 5, and 7 when PEI is being calculated</t>
-  </si>
-  <si>
-    <t>Enter only if Section 3, when PEI is being calculated</t>
   </si>
   <si>
     <t>Only used when pump can be tested at 120% BEP</t>
@@ -850,12 +833,41 @@
   <si>
     <t>pei_entry</t>
   </si>
+  <si>
+    <t>Motor Type</t>
+  </si>
+  <si>
+    <t>Polyphase Electric Motor
+Single-Phase Induction Motor
+Inverter Only Synchronous Electric Motor</t>
+  </si>
+  <si>
+    <t>Pump Configuration</t>
+  </si>
+  <si>
+    <t>Polyphase Electric Motor</t>
+  </si>
+  <si>
+    <t>Single-Phase Induction Motor</t>
+  </si>
+  <si>
+    <t>Inverter Only Synchronous Electric Motor</t>
+  </si>
+  <si>
+    <t>Pump Listing Status</t>
+  </si>
+  <si>
+    <t>Rating ID</t>
+  </si>
+  <si>
+    <t>Listing Date</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -944,8 +956,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1006,8 +1040,14 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="30">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -1057,17 +1097,6 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
       <right/>
       <top/>
       <bottom/>
@@ -1285,19 +1314,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color auto="1"/>
       </left>
@@ -1351,22 +1367,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1376,76 +1395,64 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1469,118 +1476,109 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1608,46 +1606,78 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="11" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="11" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1656,31 +1686,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2017,631 +2027,629 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AP13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AQ13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="AI4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="J4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AJ5" sqref="AJ5"/>
+      <selection pane="bottomRight" activeCell="AP1" sqref="AP1:AP2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" customWidth="1"/>
-    <col min="2" max="2" width="27.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.1640625" customWidth="1"/>
-    <col min="4" max="4" width="52.1640625" customWidth="1"/>
-    <col min="5" max="5" width="49.83203125" customWidth="1"/>
-    <col min="6" max="6" width="60.83203125" customWidth="1"/>
-    <col min="7" max="7" width="44.6640625" customWidth="1"/>
-    <col min="8" max="8" width="33.1640625" customWidth="1"/>
-    <col min="9" max="9" width="73.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" customWidth="1"/>
+    <col min="4" max="4" width="52.140625" customWidth="1"/>
+    <col min="5" max="5" width="49.85546875" customWidth="1"/>
+    <col min="6" max="6" width="60.85546875" customWidth="1"/>
+    <col min="7" max="7" width="44.7109375" customWidth="1"/>
+    <col min="8" max="8" width="33.140625" customWidth="1"/>
+    <col min="9" max="9" width="73.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="63" customWidth="1"/>
-    <col min="11" max="11" width="37.83203125" customWidth="1"/>
-    <col min="12" max="12" width="34.6640625" customWidth="1"/>
-    <col min="13" max="13" width="29" customWidth="1"/>
-    <col min="14" max="14" width="25.83203125" customWidth="1"/>
-    <col min="15" max="15" width="39.6640625" customWidth="1"/>
-    <col min="16" max="16" width="54.1640625" style="2" customWidth="1"/>
-    <col min="17" max="17" width="11" style="1" customWidth="1"/>
-    <col min="18" max="20" width="11" customWidth="1"/>
-    <col min="21" max="21" width="11" style="3" customWidth="1"/>
-    <col min="22" max="22" width="11" customWidth="1"/>
-    <col min="23" max="23" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="0" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="0" style="4" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="0" style="5" hidden="1" customWidth="1"/>
-    <col min="27" max="27" width="11" style="1" customWidth="1"/>
-    <col min="28" max="28" width="11" style="6" customWidth="1"/>
-    <col min="29" max="29" width="11" style="4" customWidth="1"/>
-    <col min="30" max="30" width="11" customWidth="1"/>
-    <col min="31" max="31" width="11" style="3" customWidth="1"/>
-    <col min="32" max="32" width="11" style="1" customWidth="1"/>
-    <col min="33" max="34" width="11" customWidth="1"/>
-    <col min="35" max="35" width="11" style="3" customWidth="1"/>
-    <col min="36" max="36" width="39.6640625" style="1" customWidth="1"/>
-    <col min="37" max="37" width="11" style="1" customWidth="1"/>
-    <col min="38" max="39" width="11" customWidth="1"/>
-    <col min="40" max="40" width="11" style="3" customWidth="1"/>
-    <col min="41" max="41" width="50" style="2" customWidth="1"/>
-    <col min="42" max="42" width="18.6640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="37.85546875" customWidth="1"/>
+    <col min="12" max="13" width="34.7109375" customWidth="1"/>
+    <col min="14" max="14" width="29" customWidth="1"/>
+    <col min="15" max="15" width="25.85546875" customWidth="1"/>
+    <col min="16" max="16" width="39.7109375" customWidth="1"/>
+    <col min="17" max="17" width="54.140625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="11" style="1" customWidth="1"/>
+    <col min="19" max="21" width="11" customWidth="1"/>
+    <col min="22" max="22" width="11" style="3" customWidth="1"/>
+    <col min="23" max="23" width="11" customWidth="1"/>
+    <col min="24" max="24" width="11" style="1" customWidth="1"/>
+    <col min="25" max="25" width="11" style="5" customWidth="1"/>
+    <col min="26" max="26" width="11" style="4" customWidth="1"/>
+    <col min="27" max="27" width="11" customWidth="1"/>
+    <col min="28" max="28" width="11" style="3" customWidth="1"/>
+    <col min="29" max="29" width="11" style="1" customWidth="1"/>
+    <col min="30" max="31" width="11" customWidth="1"/>
+    <col min="32" max="32" width="11" style="3" customWidth="1"/>
+    <col min="33" max="33" width="39.7109375" style="1" customWidth="1"/>
+    <col min="34" max="34" width="11" style="1" customWidth="1"/>
+    <col min="35" max="36" width="11" customWidth="1"/>
+    <col min="37" max="37" width="11" style="3" customWidth="1"/>
+    <col min="38" max="38" width="50" style="2" customWidth="1"/>
+    <col min="39" max="39" width="18.7109375" style="2" customWidth="1"/>
+    <col min="40" max="42" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" s="86" customFormat="1" ht="128.25" customHeight="1">
-      <c r="A1" s="86" t="s">
+    <row r="1" spans="1:43" s="79" customFormat="1" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="79" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="80"/>
+      <c r="C1" s="75" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="76" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" s="76" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="76" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" s="76" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="76" t="s">
+        <v>75</v>
+      </c>
+      <c r="I1" s="76" t="s">
+        <v>77</v>
+      </c>
+      <c r="J1" s="76" t="s">
+        <v>78</v>
+      </c>
+      <c r="K1" s="76" t="s">
+        <v>79</v>
+      </c>
+      <c r="L1" s="76" t="s">
+        <v>80</v>
+      </c>
+      <c r="M1" s="76"/>
+      <c r="N1" s="76" t="s">
+        <v>82</v>
+      </c>
+      <c r="O1" s="76" t="s">
+        <v>83</v>
+      </c>
+      <c r="P1" s="76" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q1" s="78" t="s">
+        <v>85</v>
+      </c>
+      <c r="R1" s="97" t="s">
+        <v>90</v>
+      </c>
+      <c r="S1" s="98"/>
+      <c r="T1" s="98"/>
+      <c r="U1" s="98"/>
+      <c r="V1" s="98"/>
+      <c r="W1" s="98"/>
+      <c r="X1" s="98"/>
+      <c r="Y1" s="98"/>
+      <c r="Z1" s="98"/>
+      <c r="AA1" s="98"/>
+      <c r="AB1" s="98"/>
+      <c r="AC1" s="98"/>
+      <c r="AD1" s="98"/>
+      <c r="AE1" s="98"/>
+      <c r="AF1" s="99"/>
+      <c r="AG1" s="77" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="82" t="s">
+      <c r="AH1" s="97" t="s">
+        <v>96</v>
+      </c>
+      <c r="AI1" s="98"/>
+      <c r="AJ1" s="98"/>
+      <c r="AK1" s="99"/>
+      <c r="AL1" s="78" t="s">
+        <v>97</v>
+      </c>
+      <c r="AM1" s="80"/>
+      <c r="AN1" s="81"/>
+      <c r="AP1" s="80"/>
+      <c r="AQ1" s="80"/>
+    </row>
+    <row r="2" spans="1:43" s="76" customFormat="1" ht="76.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="76" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="77" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="75" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="75" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" s="75" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q2" s="78"/>
+      <c r="R2" s="94" t="s">
+        <v>92</v>
+      </c>
+      <c r="S2" s="95"/>
+      <c r="T2" s="95"/>
+      <c r="U2" s="95"/>
+      <c r="V2" s="95"/>
+      <c r="W2" s="95"/>
+      <c r="X2" s="95"/>
+      <c r="Y2" s="95"/>
+      <c r="Z2" s="95"/>
+      <c r="AA2" s="95"/>
+      <c r="AB2" s="95"/>
+      <c r="AC2" s="95"/>
+      <c r="AD2" s="95"/>
+      <c r="AE2" s="95"/>
+      <c r="AF2" s="96"/>
+      <c r="AG2" s="77" t="s">
+        <v>95</v>
+      </c>
+      <c r="AH2" s="94" t="s">
+        <v>91</v>
+      </c>
+      <c r="AI2" s="95"/>
+      <c r="AJ2" s="95"/>
+      <c r="AK2" s="96"/>
+      <c r="AL2" s="78" t="s">
+        <v>87</v>
+      </c>
+      <c r="AM2" s="77"/>
+      <c r="AN2" s="93"/>
+      <c r="AO2" s="93"/>
+      <c r="AP2" s="93"/>
+      <c r="AQ2" s="77"/>
+    </row>
+    <row r="3" spans="1:43" s="6" customFormat="1" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D1" s="83" t="s">
-        <v>79</v>
-      </c>
-      <c r="E1" s="83" t="s">
-        <v>78</v>
-      </c>
-      <c r="F1" s="83" t="s">
+      <c r="I3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="M3" s="87" t="s">
+        <v>114</v>
+      </c>
+      <c r="N3" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="O3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="P3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="R3" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="S3" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="T3" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="U3" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="V3" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="W3" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="X3" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y3" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z3" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA3" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB3" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC3" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD3" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE3" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF3" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG3" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH3" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="AI3" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="AJ3" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="AK3" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="AL3" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="AM3" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN3" s="90" t="s">
+        <v>120</v>
+      </c>
+      <c r="AO3" s="90" t="s">
+        <v>121</v>
+      </c>
+      <c r="AP3" s="90" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:43" s="31" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="32"/>
+      <c r="M4" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="N4" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="O4" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="P4" s="32"/>
+      <c r="Q4" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="R4" s="107" t="s">
+        <v>81</v>
+      </c>
+      <c r="S4" s="108"/>
+      <c r="T4" s="108"/>
+      <c r="U4" s="108"/>
+      <c r="V4" s="109"/>
+      <c r="W4" s="35"/>
+      <c r="X4" s="102" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y4" s="102"/>
+      <c r="Z4" s="102"/>
+      <c r="AA4" s="102"/>
+      <c r="AB4" s="102"/>
+      <c r="AC4" s="103" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD4" s="103"/>
+      <c r="AE4" s="103"/>
+      <c r="AF4" s="103"/>
+      <c r="AG4" s="38"/>
+      <c r="AH4" s="39"/>
+      <c r="AI4" s="40"/>
+      <c r="AJ4" s="40"/>
+      <c r="AK4" s="41"/>
+      <c r="AL4" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="AM4" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="AN4" s="91" t="s">
+        <v>40</v>
+      </c>
+      <c r="AO4" s="91" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP4" s="91" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:43" s="31" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="45" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="46" t="s">
         <v>99</v>
       </c>
-      <c r="G1" s="83" t="s">
-        <v>80</v>
-      </c>
-      <c r="H1" s="83" t="s">
-        <v>81</v>
-      </c>
-      <c r="I1" s="83" t="s">
-        <v>83</v>
-      </c>
-      <c r="J1" s="83" t="s">
-        <v>84</v>
-      </c>
-      <c r="K1" s="83" t="s">
-        <v>85</v>
-      </c>
-      <c r="L1" s="83" t="s">
-        <v>86</v>
-      </c>
-      <c r="M1" s="83" t="s">
-        <v>88</v>
-      </c>
-      <c r="N1" s="83" t="s">
-        <v>89</v>
-      </c>
-      <c r="O1" s="83" t="s">
-        <v>90</v>
-      </c>
-      <c r="P1" s="85" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q1" s="92" t="s">
-        <v>96</v>
-      </c>
-      <c r="R1" s="93"/>
-      <c r="S1" s="93"/>
-      <c r="T1" s="93"/>
-      <c r="U1" s="93"/>
-      <c r="V1" s="93"/>
-      <c r="W1" s="93"/>
-      <c r="X1" s="93"/>
-      <c r="Y1" s="93"/>
-      <c r="Z1" s="93"/>
-      <c r="AA1" s="93"/>
-      <c r="AB1" s="93"/>
-      <c r="AC1" s="93"/>
-      <c r="AD1" s="93"/>
-      <c r="AE1" s="93"/>
-      <c r="AF1" s="93"/>
-      <c r="AG1" s="93"/>
-      <c r="AH1" s="93"/>
-      <c r="AI1" s="94"/>
-      <c r="AJ1" s="84" t="s">
+      <c r="D5" s="46" t="s">
         <v>100</v>
       </c>
-      <c r="AK1" s="92" t="s">
+      <c r="E5" s="46" t="s">
+        <v>101</v>
+      </c>
+      <c r="F5" s="46" t="s">
+        <v>106</v>
+      </c>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46" t="s">
         <v>102</v>
       </c>
-      <c r="AL1" s="93"/>
-      <c r="AM1" s="93"/>
-      <c r="AN1" s="94"/>
-      <c r="AO1" s="85" t="s">
+      <c r="I5" s="46"/>
+      <c r="J5" s="46" t="s">
+        <v>104</v>
+      </c>
+      <c r="K5" s="46" t="s">
         <v>103</v>
       </c>
-      <c r="AP1" s="88"/>
+      <c r="L5" s="46" t="s">
+        <v>111</v>
+      </c>
+      <c r="M5" s="46"/>
+      <c r="N5" s="46" t="s">
+        <v>108</v>
+      </c>
+      <c r="O5" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="P5" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q5" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="R5" s="82" t="s">
+        <v>112</v>
+      </c>
+      <c r="S5" s="83"/>
+      <c r="T5" s="83"/>
+      <c r="U5" s="83"/>
+      <c r="V5" s="83"/>
+      <c r="W5" s="35"/>
+      <c r="X5" s="84"/>
+      <c r="Y5" s="85"/>
+      <c r="Z5" s="85"/>
+      <c r="AA5" s="85"/>
+      <c r="AB5" s="85"/>
+      <c r="AC5" s="86"/>
+      <c r="AD5" s="86"/>
+      <c r="AE5" s="86"/>
+      <c r="AF5" s="86"/>
+      <c r="AG5" s="38" t="s">
+        <v>113</v>
+      </c>
+      <c r="AH5" s="36"/>
+      <c r="AI5" s="37"/>
+      <c r="AJ5" s="37"/>
+      <c r="AK5" s="37"/>
+      <c r="AL5" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="AM5" s="43"/>
+      <c r="AN5" s="92"/>
+      <c r="AO5" s="92"/>
+      <c r="AP5" s="92"/>
     </row>
-    <row r="2" spans="1:42" s="83" customFormat="1" ht="76.5" customHeight="1" thickBot="1">
-      <c r="A2" s="83" t="s">
-        <v>95</v>
-      </c>
-      <c r="B2" s="84" t="s">
-        <v>77</v>
-      </c>
-      <c r="C2" s="82" t="s">
-        <v>92</v>
-      </c>
-      <c r="D2" s="82" t="s">
-        <v>92</v>
-      </c>
-      <c r="E2" s="82" t="s">
-        <v>92</v>
-      </c>
-      <c r="P2" s="85"/>
-      <c r="Q2" s="89" t="s">
+    <row r="6" spans="1:43" s="44" customFormat="1" ht="83.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="45" t="s">
         <v>98</v>
       </c>
-      <c r="R2" s="90"/>
-      <c r="S2" s="90"/>
-      <c r="T2" s="90"/>
-      <c r="U2" s="90"/>
-      <c r="V2" s="90"/>
-      <c r="W2" s="90"/>
-      <c r="X2" s="90"/>
-      <c r="Y2" s="90"/>
-      <c r="Z2" s="90"/>
-      <c r="AA2" s="90"/>
-      <c r="AB2" s="90"/>
-      <c r="AC2" s="90"/>
-      <c r="AD2" s="90"/>
-      <c r="AE2" s="90"/>
-      <c r="AF2" s="90"/>
-      <c r="AG2" s="90"/>
-      <c r="AH2" s="90"/>
-      <c r="AI2" s="91"/>
-      <c r="AJ2" s="84" t="s">
+      <c r="C6" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="E6" s="46" t="s">
         <v>101</v>
       </c>
-      <c r="AK2" s="89" t="s">
-        <v>97</v>
-      </c>
-      <c r="AL2" s="90"/>
-      <c r="AM2" s="90"/>
-      <c r="AN2" s="91"/>
-      <c r="AO2" s="85" t="s">
-        <v>93</v>
-      </c>
-      <c r="AP2" s="85"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46" t="s">
+        <v>102</v>
+      </c>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46" t="s">
+        <v>104</v>
+      </c>
+      <c r="K6" s="46" t="s">
+        <v>103</v>
+      </c>
+      <c r="L6" s="46"/>
+      <c r="M6" s="55"/>
+      <c r="N6" s="46"/>
+      <c r="O6" s="47"/>
+      <c r="P6" s="46"/>
+      <c r="Q6" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="R6" s="104" t="s">
+        <v>42</v>
+      </c>
+      <c r="S6" s="104"/>
+      <c r="T6" s="104"/>
+      <c r="U6" s="104"/>
+      <c r="V6" s="104"/>
+      <c r="W6" s="49"/>
+      <c r="X6" s="50"/>
+      <c r="Y6" s="105" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z6" s="105"/>
+      <c r="AA6" s="105" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB6" s="105"/>
+      <c r="AC6" s="106"/>
+      <c r="AD6" s="106"/>
+      <c r="AE6" s="106"/>
+      <c r="AF6" s="106"/>
+      <c r="AG6" s="51"/>
+      <c r="AH6" s="100" t="s">
+        <v>43</v>
+      </c>
+      <c r="AI6" s="100"/>
+      <c r="AJ6" s="101" t="s">
+        <v>44</v>
+      </c>
+      <c r="AK6" s="101"/>
+      <c r="AL6" s="52"/>
+      <c r="AM6" s="53"/>
+      <c r="AN6" s="92"/>
+      <c r="AO6" s="92"/>
+      <c r="AP6" s="92"/>
     </row>
-    <row r="3" spans="1:42" s="7" customFormat="1" ht="76.5" customHeight="1">
-      <c r="B3" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="K3" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="L3" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="M3" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="N3" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="O3" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="P3" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q3" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="R3" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="S3" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="T3" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="U3" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="V3" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="W3" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="X3" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="Y3" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="Z3" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA3" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="AB3" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="AC3" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="AD3" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="AE3" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="AF3" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="AG3" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="AH3" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="AI3" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="AJ3" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="AK3" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="AL3" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="AM3" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="AN3" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="AO3" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="AP3" s="34" t="s">
-        <v>38</v>
-      </c>
+    <row r="7" spans="1:43" s="54" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="55"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="55" t="s">
+        <v>45</v>
+      </c>
+      <c r="I7" s="55"/>
+      <c r="J7" s="55"/>
+      <c r="K7" s="55"/>
+      <c r="L7" s="55" t="s">
+        <v>45</v>
+      </c>
+      <c r="M7" s="55"/>
+      <c r="N7" s="55"/>
+      <c r="O7" s="56"/>
+      <c r="P7" s="56" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q7" s="57"/>
+      <c r="R7" s="58" t="s">
+        <v>47</v>
+      </c>
+      <c r="S7" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="T7" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="U7" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="V7" s="60" t="s">
+        <v>47</v>
+      </c>
+      <c r="W7" s="61" t="s">
+        <v>48</v>
+      </c>
+      <c r="X7" s="64" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y7" s="65" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z7" s="65" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA7" s="65" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB7" s="66" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC7" s="67" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD7" s="68" t="s">
+        <v>46</v>
+      </c>
+      <c r="AE7" s="68" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF7" s="68" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG7" s="69"/>
+      <c r="AH7" s="62" t="s">
+        <v>48</v>
+      </c>
+      <c r="AI7" s="63" t="s">
+        <v>48</v>
+      </c>
+      <c r="AJ7" s="63" t="s">
+        <v>48</v>
+      </c>
+      <c r="AK7" s="70" t="s">
+        <v>48</v>
+      </c>
+      <c r="AL7" s="71"/>
+      <c r="AM7" s="72"/>
     </row>
-    <row r="4" spans="1:42" s="35" customFormat="1" ht="99" customHeight="1">
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="37" t="s">
-        <v>39</v>
-      </c>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="36"/>
-      <c r="L4" s="36"/>
-      <c r="M4" s="36" t="s">
-        <v>40</v>
-      </c>
-      <c r="N4" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="O4" s="36"/>
-      <c r="P4" s="38" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q4" s="103" t="s">
-        <v>87</v>
-      </c>
-      <c r="R4" s="104"/>
-      <c r="S4" s="104"/>
-      <c r="T4" s="104"/>
-      <c r="U4" s="105"/>
-      <c r="V4" s="39"/>
-      <c r="W4" s="40"/>
-      <c r="X4" s="41"/>
-      <c r="Y4" s="41"/>
-      <c r="Z4" s="42"/>
-      <c r="AA4" s="97" t="s">
-        <v>74</v>
-      </c>
-      <c r="AB4" s="97"/>
-      <c r="AC4" s="97"/>
-      <c r="AD4" s="97"/>
-      <c r="AE4" s="97"/>
-      <c r="AF4" s="98" t="s">
-        <v>75</v>
-      </c>
-      <c r="AG4" s="98"/>
-      <c r="AH4" s="98"/>
-      <c r="AI4" s="98"/>
-      <c r="AJ4" s="43"/>
-      <c r="AK4" s="44"/>
-      <c r="AL4" s="45"/>
-      <c r="AM4" s="45"/>
-      <c r="AN4" s="46"/>
-      <c r="AO4" s="47" t="s">
-        <v>43</v>
-      </c>
-      <c r="AP4" s="48" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:42" s="35" customFormat="1" ht="99" customHeight="1">
-      <c r="B5" s="50" t="s">
-        <v>104</v>
-      </c>
-      <c r="C5" s="51" t="s">
-        <v>105</v>
-      </c>
-      <c r="D5" s="51" t="s">
-        <v>106</v>
-      </c>
-      <c r="E5" s="51" t="s">
-        <v>107</v>
-      </c>
-      <c r="F5" s="51" t="s">
-        <v>112</v>
-      </c>
-      <c r="G5" s="51"/>
-      <c r="H5" s="51" t="s">
-        <v>108</v>
-      </c>
-      <c r="I5" s="51"/>
-      <c r="J5" s="51" t="s">
-        <v>110</v>
-      </c>
-      <c r="K5" s="51" t="s">
-        <v>109</v>
-      </c>
-      <c r="L5" s="51" t="s">
-        <v>117</v>
-      </c>
-      <c r="M5" s="51" t="s">
-        <v>114</v>
-      </c>
-      <c r="N5" s="52" t="s">
-        <v>115</v>
-      </c>
-      <c r="O5" s="51" t="s">
-        <v>113</v>
-      </c>
-      <c r="P5" s="38" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q5" s="106" t="s">
-        <v>118</v>
-      </c>
-      <c r="R5" s="107"/>
-      <c r="S5" s="107"/>
-      <c r="T5" s="107"/>
-      <c r="U5" s="107"/>
-      <c r="V5" s="39"/>
-      <c r="W5" s="40"/>
-      <c r="X5" s="41"/>
-      <c r="Y5" s="41"/>
-      <c r="Z5" s="42"/>
-      <c r="AA5" s="108"/>
-      <c r="AB5" s="109"/>
-      <c r="AC5" s="109"/>
-      <c r="AD5" s="109"/>
-      <c r="AE5" s="109"/>
-      <c r="AF5" s="110"/>
-      <c r="AG5" s="110"/>
-      <c r="AH5" s="110"/>
-      <c r="AI5" s="110"/>
-      <c r="AJ5" s="43" t="s">
-        <v>119</v>
-      </c>
-      <c r="AK5" s="40"/>
-      <c r="AL5" s="111"/>
-      <c r="AM5" s="111"/>
-      <c r="AN5" s="111"/>
-      <c r="AO5" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="AP5" s="48"/>
-    </row>
-    <row r="6" spans="1:42" s="49" customFormat="1" ht="83" customHeight="1" thickBot="1">
-      <c r="B6" s="50" t="s">
-        <v>104</v>
-      </c>
-      <c r="C6" s="51" t="s">
-        <v>105</v>
-      </c>
-      <c r="D6" s="51" t="s">
-        <v>106</v>
-      </c>
-      <c r="E6" s="51" t="s">
-        <v>107</v>
-      </c>
-      <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
-      <c r="H6" s="51" t="s">
-        <v>108</v>
-      </c>
-      <c r="I6" s="51"/>
-      <c r="J6" s="51" t="s">
-        <v>110</v>
-      </c>
-      <c r="K6" s="51" t="s">
-        <v>109</v>
-      </c>
-      <c r="L6" s="51"/>
-      <c r="M6" s="51"/>
-      <c r="N6" s="52"/>
-      <c r="O6" s="51"/>
-      <c r="P6" s="53" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q6" s="99" t="s">
-        <v>46</v>
-      </c>
-      <c r="R6" s="99"/>
-      <c r="S6" s="99"/>
-      <c r="T6" s="99"/>
-      <c r="U6" s="99"/>
-      <c r="V6" s="54"/>
-      <c r="W6" s="100" t="s">
-        <v>47</v>
-      </c>
-      <c r="X6" s="100"/>
-      <c r="Y6" s="100"/>
-      <c r="Z6" s="55" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA6" s="56"/>
-      <c r="AB6" s="101" t="s">
+    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AC6" s="101"/>
-      <c r="AD6" s="101" t="s">
+      <c r="C8" t="s">
         <v>50</v>
       </c>
-      <c r="AE6" s="101"/>
-      <c r="AF6" s="102"/>
-      <c r="AG6" s="102"/>
-      <c r="AH6" s="102"/>
-      <c r="AI6" s="102"/>
-      <c r="AJ6" s="57"/>
-      <c r="AK6" s="95" t="s">
-        <v>49</v>
-      </c>
-      <c r="AL6" s="95"/>
-      <c r="AM6" s="96" t="s">
-        <v>50</v>
-      </c>
-      <c r="AN6" s="96"/>
-      <c r="AO6" s="58"/>
-      <c r="AP6" s="59"/>
-    </row>
-    <row r="7" spans="1:42" s="60" customFormat="1" ht="23" customHeight="1">
-      <c r="B7" s="61"/>
-      <c r="C7" s="61"/>
-      <c r="D7" s="61"/>
-      <c r="E7" s="61"/>
-      <c r="F7" s="61"/>
-      <c r="G7" s="61"/>
-      <c r="H7" s="61" t="s">
-        <v>51</v>
-      </c>
-      <c r="I7" s="61"/>
-      <c r="J7" s="61"/>
-      <c r="K7" s="61"/>
-      <c r="L7" s="61" t="s">
-        <v>51</v>
-      </c>
-      <c r="M7" s="61"/>
-      <c r="N7" s="62"/>
-      <c r="O7" s="62" t="s">
-        <v>52</v>
-      </c>
-      <c r="P7" s="63"/>
-      <c r="Q7" s="64" t="s">
-        <v>53</v>
-      </c>
-      <c r="R7" s="65" t="s">
-        <v>53</v>
-      </c>
-      <c r="S7" s="65" t="s">
-        <v>53</v>
-      </c>
-      <c r="T7" s="65" t="s">
-        <v>53</v>
-      </c>
-      <c r="U7" s="66" t="s">
-        <v>53</v>
-      </c>
-      <c r="V7" s="67" t="s">
-        <v>54</v>
-      </c>
-      <c r="W7" s="68"/>
-      <c r="X7" s="69"/>
-      <c r="Y7" s="69"/>
-      <c r="Z7" s="70"/>
-      <c r="AA7" s="71" t="s">
-        <v>52</v>
-      </c>
-      <c r="AB7" s="72" t="s">
-        <v>52</v>
-      </c>
-      <c r="AC7" s="72" t="s">
-        <v>52</v>
-      </c>
-      <c r="AD7" s="72" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE7" s="73" t="s">
-        <v>52</v>
-      </c>
-      <c r="AF7" s="74" t="s">
-        <v>52</v>
-      </c>
-      <c r="AG7" s="75" t="s">
-        <v>52</v>
-      </c>
-      <c r="AH7" s="75" t="s">
-        <v>52</v>
-      </c>
-      <c r="AI7" s="75" t="s">
-        <v>52</v>
-      </c>
-      <c r="AJ7" s="76"/>
-      <c r="AK7" s="68" t="s">
-        <v>54</v>
-      </c>
-      <c r="AL7" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="AM7" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="AN7" s="77" t="s">
-        <v>54</v>
-      </c>
-      <c r="AO7" s="78"/>
-      <c r="AP7" s="79"/>
-    </row>
-    <row r="8" spans="1:42">
-      <c r="B8" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>56</v>
       </c>
-      <c r="D8" t="s">
-        <v>62</v>
-      </c>
       <c r="E8" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="F8" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="G8" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="H8">
         <v>10</v>
@@ -2655,65 +2663,65 @@
       <c r="K8">
         <v>3600</v>
       </c>
-      <c r="M8" t="s">
-        <v>65</v>
-      </c>
-      <c r="N8">
+      <c r="N8" t="s">
+        <v>59</v>
+      </c>
+      <c r="O8">
         <v>95</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <v>60</v>
       </c>
-      <c r="P8" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q8" s="1">
+      <c r="Q8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="R8" s="1">
         <v>349.83049999999997</v>
       </c>
-      <c r="V8">
+      <c r="W8">
         <v>424.4298</v>
       </c>
-      <c r="AA8" s="1">
+      <c r="X8" s="1">
         <v>59.0717</v>
       </c>
-      <c r="AB8" s="6">
+      <c r="Y8" s="5">
         <v>56.555799999999998</v>
       </c>
-      <c r="AC8" s="4">
+      <c r="Z8" s="4">
         <v>59.491</v>
       </c>
-      <c r="AJ8" s="1">
+      <c r="AG8" s="1">
         <v>0.9</v>
       </c>
-      <c r="AK8" s="1">
+      <c r="AH8" s="1">
         <v>498.89100000000002</v>
       </c>
-      <c r="AL8">
+      <c r="AI8">
         <v>383.476</v>
       </c>
-      <c r="AN8" s="80"/>
-      <c r="AO8" s="2">
+      <c r="AK8" s="73"/>
+      <c r="AL8" s="2">
         <v>106</v>
       </c>
     </row>
-    <row r="9" spans="1:42">
+    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" t="s">
         <v>56</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>62</v>
       </c>
-      <c r="E9" t="s">
-        <v>68</v>
-      </c>
       <c r="F9" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="G9" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="H9">
         <v>10</v>
@@ -2727,64 +2735,64 @@
       <c r="K9">
         <v>3600</v>
       </c>
-      <c r="M9" t="s">
-        <v>65</v>
-      </c>
-      <c r="N9">
+      <c r="N9" t="s">
+        <v>59</v>
+      </c>
+      <c r="O9">
         <v>96</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <v>60</v>
       </c>
-      <c r="P9" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q9" s="1">
+      <c r="Q9" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="R9" s="1">
         <v>349.83049999999997</v>
       </c>
-      <c r="V9">
+      <c r="W9">
         <v>424.4298</v>
       </c>
-      <c r="AA9" s="1">
+      <c r="X9" s="1">
         <v>59.0717</v>
       </c>
-      <c r="AB9" s="6">
+      <c r="Y9" s="5">
         <v>56.555799999999998</v>
       </c>
-      <c r="AC9" s="4">
+      <c r="Z9" s="4">
         <v>59.491</v>
       </c>
-      <c r="AJ9" s="1">
+      <c r="AG9" s="1">
         <v>0.9</v>
       </c>
-      <c r="AK9" s="1">
+      <c r="AH9" s="1">
         <v>498.89100000000002</v>
       </c>
-      <c r="AL9">
+      <c r="AI9">
         <v>383.476</v>
       </c>
-      <c r="AO9" s="2">
+      <c r="AL9" s="2">
         <v>106</v>
       </c>
     </row>
-    <row r="10" spans="1:42">
+    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" t="s">
         <v>56</v>
       </c>
-      <c r="D10" t="s">
-        <v>62</v>
-      </c>
       <c r="E10" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F10" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="G10" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="H10">
         <v>10</v>
@@ -2798,64 +2806,64 @@
       <c r="K10">
         <v>3600</v>
       </c>
-      <c r="M10" t="s">
-        <v>65</v>
-      </c>
-      <c r="N10">
+      <c r="N10" t="s">
+        <v>59</v>
+      </c>
+      <c r="O10">
         <v>97</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <v>60</v>
       </c>
-      <c r="P10" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q10" s="1">
+      <c r="Q10" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="R10" s="1">
         <v>349.83049999999997</v>
       </c>
-      <c r="V10">
+      <c r="W10">
         <v>424.4298</v>
       </c>
-      <c r="AA10" s="1">
+      <c r="X10" s="1">
         <v>59.0717</v>
       </c>
-      <c r="AB10" s="6">
+      <c r="Y10" s="5">
         <v>56.555799999999998</v>
       </c>
-      <c r="AC10" s="4">
+      <c r="Z10" s="4">
         <v>59.491</v>
       </c>
-      <c r="AJ10" s="1">
+      <c r="AG10" s="1">
         <v>0.9</v>
       </c>
-      <c r="AK10" s="1">
+      <c r="AH10" s="1">
         <v>498.89100000000002</v>
       </c>
-      <c r="AL10">
+      <c r="AI10">
         <v>383.476</v>
       </c>
-      <c r="AO10" s="2">
+      <c r="AL10" s="2">
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:42">
+    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" t="s">
         <v>56</v>
       </c>
-      <c r="D11" t="s">
-        <v>62</v>
-      </c>
       <c r="E11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F11" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="G11" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="H11">
         <v>10</v>
@@ -2869,64 +2877,64 @@
       <c r="K11">
         <v>3600</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
+        <v>59</v>
+      </c>
+      <c r="O11">
+        <v>95</v>
+      </c>
+      <c r="P11">
+        <v>75</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="R11" s="1">
+        <v>349.83049999999997</v>
+      </c>
+      <c r="W11">
+        <v>424.4298</v>
+      </c>
+      <c r="X11" s="1">
+        <v>59.0717</v>
+      </c>
+      <c r="Y11" s="5">
+        <v>56.555799999999998</v>
+      </c>
+      <c r="Z11" s="4">
+        <v>59.491</v>
+      </c>
+      <c r="AG11" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="AH11" s="1">
+        <v>498.89100000000002</v>
+      </c>
+      <c r="AI11">
+        <v>383.476</v>
+      </c>
+      <c r="AL11" s="2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" t="s">
         <v>65</v>
       </c>
-      <c r="N11">
-        <v>95</v>
-      </c>
-      <c r="O11">
-        <v>75</v>
-      </c>
-      <c r="P11" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q11" s="1">
-        <v>349.83049999999997</v>
-      </c>
-      <c r="V11">
-        <v>424.4298</v>
-      </c>
-      <c r="AA11" s="1">
-        <v>59.0717</v>
-      </c>
-      <c r="AB11" s="6">
-        <v>56.555799999999998</v>
-      </c>
-      <c r="AC11" s="4">
-        <v>59.491</v>
-      </c>
-      <c r="AJ11" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="AK11" s="1">
-        <v>498.89100000000002</v>
-      </c>
-      <c r="AL11">
-        <v>383.476</v>
-      </c>
-      <c r="AO11" s="2">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="12" spans="1:42">
-      <c r="B12" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C12" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" t="s">
-        <v>62</v>
-      </c>
-      <c r="E12" t="s">
-        <v>71</v>
-      </c>
       <c r="F12" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="G12" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="H12">
         <v>10</v>
@@ -2940,67 +2948,67 @@
       <c r="K12">
         <v>3600</v>
       </c>
-      <c r="M12" t="s">
-        <v>65</v>
-      </c>
-      <c r="N12">
+      <c r="N12" t="s">
+        <v>59</v>
+      </c>
+      <c r="O12">
         <v>96</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <v>75</v>
       </c>
-      <c r="P12" s="2" t="s">
+      <c r="Q12" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="R12" s="1">
+        <v>349.83049999999997</v>
+      </c>
+      <c r="W12">
+        <v>424.4298</v>
+      </c>
+      <c r="X12" s="1">
+        <v>59.0717</v>
+      </c>
+      <c r="Y12" s="5">
+        <v>56.555799999999998</v>
+      </c>
+      <c r="Z12" s="4">
+        <v>59.491</v>
+      </c>
+      <c r="AG12" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="AH12" s="1">
+        <v>498.89100000000002</v>
+      </c>
+      <c r="AI12">
+        <v>383.476</v>
+      </c>
+      <c r="AJ12" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL12" s="2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" t="s">
         <v>66</v>
       </c>
-      <c r="Q12" s="1">
-        <v>349.83049999999997</v>
-      </c>
-      <c r="V12">
-        <v>424.4298</v>
-      </c>
-      <c r="AA12" s="1">
-        <v>59.0717</v>
-      </c>
-      <c r="AB12" s="6">
-        <v>56.555799999999998</v>
-      </c>
-      <c r="AC12" s="4">
-        <v>59.491</v>
-      </c>
-      <c r="AJ12" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="AK12" s="1">
-        <v>498.89100000000002</v>
-      </c>
-      <c r="AL12">
-        <v>383.476</v>
-      </c>
-      <c r="AM12" t="s">
+      <c r="F13" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" t="s">
         <v>58</v>
-      </c>
-      <c r="AO12" s="2">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="13" spans="1:42">
-      <c r="B13" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" t="s">
-        <v>56</v>
-      </c>
-      <c r="D13" t="s">
-        <v>62</v>
-      </c>
-      <c r="E13" t="s">
-        <v>72</v>
-      </c>
-      <c r="F13" t="s">
-        <v>63</v>
-      </c>
-      <c r="G13" t="s">
-        <v>64</v>
       </c>
       <c r="H13">
         <v>10</v>
@@ -3014,66 +3022,65 @@
       <c r="K13">
         <v>3600</v>
       </c>
-      <c r="M13" t="s">
-        <v>65</v>
-      </c>
-      <c r="N13">
+      <c r="N13" t="s">
+        <v>59</v>
+      </c>
+      <c r="O13">
         <v>97</v>
       </c>
-      <c r="O13">
+      <c r="P13">
         <v>75</v>
       </c>
-      <c r="P13" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q13" s="1">
+      <c r="Q13" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="R13" s="1">
         <v>349.83049999999997</v>
       </c>
-      <c r="V13">
+      <c r="W13">
         <v>424.4298</v>
       </c>
-      <c r="AA13" s="1">
+      <c r="X13" s="1">
         <v>59.0717</v>
       </c>
-      <c r="AB13" s="6">
+      <c r="Y13" s="5">
         <v>56.555799999999998</v>
       </c>
-      <c r="AC13" s="4">
+      <c r="Z13" s="4">
         <v>59.491</v>
       </c>
-      <c r="AJ13" s="1">
+      <c r="AG13" s="1">
         <v>0.9</v>
       </c>
-      <c r="AK13" s="1">
+      <c r="AH13" s="1">
         <v>498.89100000000002</v>
       </c>
-      <c r="AL13">
+      <c r="AI13">
         <v>383.476</v>
       </c>
-      <c r="AO13" s="2">
+      <c r="AL13" s="2">
         <v>106</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="AK2:AN2"/>
-    <mergeCell ref="AK1:AN1"/>
-    <mergeCell ref="Q1:AI1"/>
-    <mergeCell ref="Q2:AI2"/>
-    <mergeCell ref="AK6:AL6"/>
-    <mergeCell ref="AM6:AN6"/>
-    <mergeCell ref="AA4:AE4"/>
-    <mergeCell ref="AF4:AI4"/>
-    <mergeCell ref="Q6:U6"/>
-    <mergeCell ref="W6:Y6"/>
-    <mergeCell ref="AB6:AC6"/>
-    <mergeCell ref="AD6:AE6"/>
-    <mergeCell ref="AF6:AI6"/>
-    <mergeCell ref="Q4:U4"/>
+  <mergeCells count="13">
+    <mergeCell ref="AH2:AK2"/>
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="R1:AF1"/>
+    <mergeCell ref="R2:AF2"/>
+    <mergeCell ref="AH6:AI6"/>
+    <mergeCell ref="AJ6:AK6"/>
+    <mergeCell ref="X4:AB4"/>
+    <mergeCell ref="AC4:AF4"/>
+    <mergeCell ref="R6:V6"/>
+    <mergeCell ref="Y6:Z6"/>
+    <mergeCell ref="AA6:AB6"/>
+    <mergeCell ref="AC6:AF6"/>
+    <mergeCell ref="R4:V4"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3083,31 +3090,58 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7:G8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="15">
-      <c r="A1" s="81" t="s">
-        <v>57</v>
+    <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="88" t="s">
+        <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15">
-      <c r="A2" s="81" t="s">
-        <v>59</v>
+    <row r="2" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="74" t="s">
+        <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15">
-      <c r="A3" s="81" t="s">
-        <v>60</v>
+    <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="74" t="s">
+        <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15">
-      <c r="A4" s="81" t="s">
-        <v>61</v>
+    <row r="4" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="74" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="74" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="89" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>